<commit_message>
Omitted Enterobacter from core essentials
</commit_message>
<xml_diff>
--- a/core-essential.xlsx
+++ b/core-essential.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="50">
   <si>
     <t>Core essentials defined using 80% threshold</t>
   </si>
@@ -35,25 +35,124 @@
     <t>Cell Division</t>
   </si>
   <si>
+    <t>ftsAHQWYZ, mukB, zipA</t>
+  </si>
+  <si>
+    <t>ftsJKLNX, cedA, minCDE, sdiA, sulA</t>
+  </si>
+  <si>
+    <t>DNA Replication</t>
+  </si>
+  <si>
+    <t>Polymerases I, II and III</t>
+  </si>
+  <si>
+    <t>dnaENQX, holAB</t>
+  </si>
+  <si>
+    <t>holCDE, polAB</t>
+  </si>
+  <si>
+    <t>Supercoiling</t>
+  </si>
+  <si>
+    <t>gyrAB, parCE</t>
+  </si>
+  <si>
+    <t>Primosome Associated</t>
+  </si>
+  <si>
+    <t>dnaBCGT, priA, ssb</t>
+  </si>
+  <si>
+    <t>priBC, rep</t>
+  </si>
+  <si>
+    <t>Transcription</t>
+  </si>
+  <si>
+    <t>RNA Polymerase</t>
+  </si>
+  <si>
+    <t>rpoABC</t>
+  </si>
+  <si>
+    <t>Sigma, Elongation, Anti- and Termination Factors</t>
+  </si>
+  <si>
+    <t>nusABG, rpoDH, rho</t>
+  </si>
+  <si>
+    <t>rpoENS</t>
+  </si>
+  <si>
+    <t>Translation</t>
+  </si>
+  <si>
+    <t>tRNA Synthetases</t>
+  </si>
+  <si>
+    <t>alaS, argS, asnS, aspS, cysS, glnS, gltX, glyQS, hisS, ileS, leuS, lysS, metG, pheST, proS, serS, thrS, tyrS, valS</t>
+  </si>
+  <si>
+    <t>trpS</t>
+  </si>
+  <si>
+    <t>Ribosome Components</t>
+  </si>
+  <si>
+    <t>rplBCDEFJKLMNOPQRSTUVWXY, rpmABCDH, rpsABCDEGHJKLMNPQRSTU</t>
+  </si>
+  <si>
+    <t>rplAI, rpmEFGIJJ2, rpsFIOV</t>
+  </si>
+  <si>
+    <t>Initiation, elongation and peptide chain release factors</t>
+  </si>
+  <si>
+    <t>fusA, infABC, prfAB, tsf, yrdC</t>
+  </si>
+  <si>
+    <t>efp, prfCH, selB, tuf</t>
+  </si>
+  <si>
+    <t>Biosynthetic Pathways</t>
+  </si>
+  <si>
+    <t>Peptidoglycan</t>
+  </si>
+  <si>
+    <t>murABCDEFGI</t>
+  </si>
+  <si>
+    <t>ddlAB</t>
+  </si>
+  <si>
+    <t>Fatty Acids</t>
+  </si>
+  <si>
+    <t>accABCD, fabABDGHIZ</t>
+  </si>
+  <si>
+    <t>Ancestrally essentials defined using Fitch's algorithm</t>
+  </si>
+  <si>
+    <t>Ancestrally Essential</t>
+  </si>
+  <si>
+    <t>Not Ancestrally Essential</t>
+  </si>
+  <si>
     <t>ftsAHLQWYZ, minE, mukB, zipA</t>
   </si>
   <si>
     <t>ftsJKNX, cedA, minCD, sdiA, sulA</t>
   </si>
   <si>
-    <t>DNA Replication</t>
-  </si>
-  <si>
-    <t>Polymerases I, II and III</t>
-  </si>
-  <si>
-    <t>dnaENQX, holABC, polA</t>
-  </si>
-  <si>
-    <t>holDE, polB</t>
-  </si>
-  <si>
-    <t>Supercoiling</t>
+    <t>dnaENQX, holABD</t>
+  </si>
+  <si>
+    <t>holCE, polAB</t>
   </si>
   <si>
     <t>gyrAB, parE</t>
@@ -62,94 +161,10 @@
     <t>parC</t>
   </si>
   <si>
-    <t>Primosome Associated</t>
-  </si>
-  <si>
-    <t>dnaBCGT, priA, ssb</t>
-  </si>
-  <si>
-    <t>priBC, rep</t>
-  </si>
-  <si>
-    <t>Transcription</t>
-  </si>
-  <si>
-    <t>RNA Polymerase</t>
-  </si>
-  <si>
-    <t>rpoABC</t>
-  </si>
-  <si>
-    <t>Sigma, Elongation, Anti- and Termination Factors</t>
-  </si>
-  <si>
-    <t>nusABG, rpoDH, rho</t>
-  </si>
-  <si>
-    <t>rpoENS</t>
-  </si>
-  <si>
-    <t>Translation</t>
-  </si>
-  <si>
-    <t>tRNA Synthetases</t>
-  </si>
-  <si>
-    <t>alaS, argS, asnS, aspS, cysS, glnS, gltX, glyQS, hisS, ileS, leuS, lysS, metG, pheST, proS, serS, thrS, tyrS, valS</t>
-  </si>
-  <si>
-    <t>trpS</t>
-  </si>
-  <si>
-    <t>Ribosome Components</t>
-  </si>
-  <si>
-    <t>rplBCDEFJKLMNOPQRSTUVWXY, rpmABCDH, rpsABCDEGHJKLMNPQRSTU</t>
-  </si>
-  <si>
-    <t>rplAI, rmpEFGIJJ2, rpsFIOV</t>
-  </si>
-  <si>
-    <t>Initiation, elongation and peptide chain release factors</t>
-  </si>
-  <si>
-    <t>fusA, infABC, prfAB, tsf, yrdC</t>
-  </si>
-  <si>
-    <t>efp, prfCH, selB, tuf</t>
-  </si>
-  <si>
-    <t>Biosynthetic Pathways</t>
-  </si>
-  <si>
-    <t>Peptidoglycan</t>
-  </si>
-  <si>
-    <t>murABCDEFGI</t>
-  </si>
-  <si>
-    <t>ddlAB</t>
-  </si>
-  <si>
-    <t>Fatty Acids</t>
-  </si>
-  <si>
-    <t>accABCD, fabABDGHIZ</t>
-  </si>
-  <si>
-    <t>Ancestrally essentials defined using Fitch's algorithm</t>
-  </si>
-  <si>
-    <t>Ancestrally Essential</t>
-  </si>
-  <si>
-    <t>Not Ancestrally Essential</t>
-  </si>
-  <si>
-    <t>rplABCDEFJKLMNOPQRSTUVWXY, rpmABCDH, rpsABCDEFGHJKLMNOPQRSTU</t>
-  </si>
-  <si>
-    <t>rplI, rmpEFGIJJ2, rpsIV</t>
+    <t>rplABCDEFJKLMNOPQRSTUVWXY, rpmABCDHI, rpsABCDEFGHJKLMNOPQRSTU</t>
+  </si>
+  <si>
+    <t>rplI, rpmEFGJJ2, rpsIV</t>
   </si>
 </sst>
 </file>
@@ -268,9 +283,9 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
+      <selection pane="bottomLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -343,105 +358,102 @@
       <c r="C6" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0"/>
       <c r="B7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="D7" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="C8" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0"/>
       <c r="B9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="D9" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="C10" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="D10" s="0" t="s">
         <v>26</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0"/>
       <c r="B11" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="D11" s="0" t="s">
         <v>29</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0"/>
       <c r="B12" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="D12" s="0" t="s">
         <v>32</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="D14" s="0" t="s">
         <v>36</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="0" t="s">
         <v>38</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -452,7 +464,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -472,10 +484,10 @@
         <v>2</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -483,10 +495,10 @@
         <v>5</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -497,10 +509,10 @@
         <v>9</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -509,107 +521,107 @@
         <v>12</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0"/>
       <c r="B24" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="D24" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="C25" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0"/>
       <c r="B26" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="D26" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="C27" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="D27" s="0" t="s">
         <v>26</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0"/>
       <c r="B28" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0"/>
       <c r="B29" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="D29" s="0" t="s">
         <v>32</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="D31" s="0" t="s">
         <v>36</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="0" t="s">
         <v>38</v>
-      </c>
-      <c r="C32" s="0" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added ancestrally essential to giant table, changed ancestrally essential according to new gene clustering
</commit_message>
<xml_diff>
--- a/core-essential.xlsx
+++ b/core-essential.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="133" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="121" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="50">
   <si>
     <t>Core essentials defined using 80% threshold</t>
   </si>
@@ -155,12 +155,6 @@
     <t>holCE, polAB</t>
   </si>
   <si>
-    <t>gyrAB, parE</t>
-  </si>
-  <si>
-    <t>parC</t>
-  </si>
-  <si>
     <t>rplABCDEFJKLMNOPQRSTUVWXY, rpmABCDHI, rpsABCDEFGHJKLMNOPQRSTU</t>
   </si>
   <si>
@@ -170,8 +164,7 @@
     <t>Other</t>
   </si>
   <si>
-    <t>acpPS, adk, asd, bamAD, birA, cca, cdsA, coaADE, cohE, csrA, dapABDE, def, der, dfp, dnaAK, dut, dxr, dxs, eno, era, erpA, fbaA, ffh, fldA, fmt, folABCDEK, frr, ftsBI, gapA, glmMSU, glyA, gmk, gpsA, groLS, grpE, hemABCDEGHL, iscS, ispABDEFGHU, kdsAB, lepB, lexA, lgt, ligA, lnt, lolABCDE, lpd, lptABDEFG, lpxABCDHK, lspA, metK, mnmA, mraY, mrdAB, mreBCD, msbA, mukEF, murJ, nadDEK, nrdAB, nrfF, obgE, orn, pgk, pgsA, plsBC, ppa, prs, psd, pssA, pth, pyrGH, ribABCDEF, rimM, rnc, rnpA, secADEFY, suhB, tadA, thiL, thyA, tilS, tmk, topA, trmD, tsaBDE, ubiABDEGHX, waaA, ybeY, ygfZ, yidC, yihA, yqgF
-</t>
+    <t>acpPS, adk, asd, bamAD, birA, cca, cdsA, coaADE, cohE, csrA, dapABDE, def, der, dfp, dnaAK, dut, dxr, dxs, eno, era, erpA, fbaA, ffh, fldA, fmt, folABCDEK, frr, ftsBI, gapA, glmMSU, glyA, gmk, gpsA, groLS, grpE, hemABCDEGHL, iscS, ispABDEFGHU, kdsAB, lepB, lexA, lgt, ligA, lnt, lolABCDE, lpd, lptABDEFG, lpxABCDHK, lspA, metK, mnmA, mraY, mrdAB, mreBCD, msbA, mukEF, murJ, nadDEK, nrdAB, obgE, orn, pgk, pgsA, plsBC, ppa, prs, psd, pssA, pth, pyrGH, ribABCDEF, rimM, rnc, rnpA, rodZ, secADEFY, suhB, tadA, thiL, thyA, tilS, tmk, topA, trmD, tsaBDE, ubiABDEGHX, waaA, ybeY, ygfZ, yidC, yihA, yqgF</t>
   </si>
 </sst>
 </file>
@@ -215,6 +208,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -538,10 +532,7 @@
         <v>12</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -599,10 +590,10 @@
         <v>27</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -643,10 +634,10 @@
     </row>
     <row r="33" customFormat="false" ht="70.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>